<commit_message>
Atualiza contatos.xlsx com nova versão local
</commit_message>
<xml_diff>
--- a/data/contatos.xlsx
+++ b/data/contatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Efraim\WhatsAppAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A794A91-4DF3-43AF-8F79-96FBCD98EFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9ABB86-7F66-4EEB-BDBF-A6262167B514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Maria</t>
   </si>
   <si>
-    <t>5512992087984</t>
-  </si>
-  <si>
     <t>Jose</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Abreu</t>
+  </si>
+  <si>
+    <t>5512990000000</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +433,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>"Olá "&amp; A2 &amp; ", tudo bem?"</f>
@@ -445,10 +445,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" ref="C3:C7" si="0">"Olá "&amp; A3 &amp; ", tudo bem?"</f>
@@ -457,10 +457,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -484,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -493,10 +493,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>

</xml_diff>